<commit_message>
- finish intro, updated cotton csv
</commit_message>
<xml_diff>
--- a/Data/US Econ history graphs.xlsx
+++ b/Data/US Econ history graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryo Nakagawara\Google Drive\US Econ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryo Nakagawara\Documents\R_materials\AmericaJapanPostWW2Trade\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -206,6 +206,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -478,11 +479,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="128680264"/>
-        <c:axId val="128680656"/>
+        <c:axId val="361395288"/>
+        <c:axId val="361391368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128680264"/>
+        <c:axId val="361395288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,7 +520,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128680656"/>
+        <c:crossAx val="361391368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -527,7 +528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128680656"/>
+        <c:axId val="361391368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,6 +557,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -610,7 +612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128680264"/>
+        <c:crossAx val="361395288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -696,6 +698,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1013,11 +1016,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="128681440"/>
-        <c:axId val="128681832"/>
+        <c:axId val="361397248"/>
+        <c:axId val="361393328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128681440"/>
+        <c:axId val="361397248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +1063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128681832"/>
+        <c:crossAx val="361393328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1068,7 +1071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128681832"/>
+        <c:axId val="361393328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,6 +1117,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1174,7 +1178,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128681440"/>
+        <c:crossAx val="361397248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1188,6 +1192,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1560,11 +1565,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="128682616"/>
-        <c:axId val="128683008"/>
+        <c:axId val="361392152"/>
+        <c:axId val="361393720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128682616"/>
+        <c:axId val="361392152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1607,7 +1612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128683008"/>
+        <c:crossAx val="361393720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1615,7 +1620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128683008"/>
+        <c:axId val="361393720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128682616"/>
+        <c:crossAx val="361392152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1935,11 +1940,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="128683792"/>
-        <c:axId val="128684184"/>
+        <c:axId val="361394504"/>
+        <c:axId val="361394896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128683792"/>
+        <c:axId val="361394504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,7 +1981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128684184"/>
+        <c:crossAx val="361394896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1984,7 +1989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128684184"/>
+        <c:axId val="361394896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2068,7 +2073,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128683792"/>
+        <c:crossAx val="361394504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2277,11 +2282,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="170164528"/>
-        <c:axId val="170164920"/>
+        <c:axId val="441587160"/>
+        <c:axId val="441585984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="170164528"/>
+        <c:axId val="441587160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2324,7 +2329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170164920"/>
+        <c:crossAx val="441585984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2332,7 +2337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170164920"/>
+        <c:axId val="441585984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,7 +2430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170164528"/>
+        <c:crossAx val="441587160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2859,11 +2864,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="170165704"/>
-        <c:axId val="170166096"/>
+        <c:axId val="441580496"/>
+        <c:axId val="441580888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="170165704"/>
+        <c:axId val="441580496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2906,7 +2911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170166096"/>
+        <c:crossAx val="441580888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2914,7 +2919,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170166096"/>
+        <c:axId val="441580888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3007,7 +3012,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170165704"/>
+        <c:crossAx val="441580496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3308,11 +3313,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="170317656"/>
-        <c:axId val="170318048"/>
+        <c:axId val="441581280"/>
+        <c:axId val="441581672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="170317656"/>
+        <c:axId val="441581280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3355,7 +3360,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170318048"/>
+        <c:crossAx val="441581672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3363,7 +3368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170318048"/>
+        <c:axId val="441581672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3456,7 +3461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170317656"/>
+        <c:crossAx val="441581280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3686,8 +3691,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="170318832"/>
-        <c:axId val="170319224"/>
+        <c:axId val="441582848"/>
+        <c:axId val="441584416"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3780,11 +3785,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="170320008"/>
-        <c:axId val="170319616"/>
+        <c:axId val="441579712"/>
+        <c:axId val="441583240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="170318832"/>
+        <c:axId val="441582848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3858,7 +3863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170319224"/>
+        <c:crossAx val="441584416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3866,7 +3871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170319224"/>
+        <c:axId val="441584416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3973,12 +3978,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170318832"/>
+        <c:crossAx val="441582848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170319616"/>
+        <c:axId val="441583240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4071,12 +4076,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170320008"/>
+        <c:crossAx val="441579712"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="170320008"/>
+        <c:axId val="441579712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4086,7 +4091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170319616"/>
+        <c:crossAx val="441583240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9170,8 +9175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9478,7 +9483,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>